<commit_message>
Added Scirpt for Extended Kalman filter. Appears to be tracking reference.
</commit_message>
<xml_diff>
--- a/X1_X2_X3_data.xlsx
+++ b/X1_X2_X3_data.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umd0-my.sharepoint.com/personal/ggilbert_umd_edu1/Documents/Documents/MATLAB/ENPM667/ENPM667_Project_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{78EA2A0A-57C8-4A89-9094-5E1D1EC4B199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF71AA81-E36E-4CC6-8833-068363777B3B}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="13_ncr:1_{78EA2A0A-57C8-4A89-9094-5E1D1EC4B199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B757211-5390-4854-8099-9971271A7C4D}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{19C20825-B259-453C-88C5-1721DCB93B13}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="3" xr2:uid="{19C20825-B259-453C-88C5-1721DCB93B13}"/>
   </bookViews>
   <sheets>
     <sheet name="x1" sheetId="1" r:id="rId1"/>
     <sheet name="x2" sheetId="2" r:id="rId2"/>
     <sheet name="x3" sheetId="3" r:id="rId3"/>
+    <sheet name="psi_k" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -6357,7 +6358,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F5BF7B6-BE96-4980-B1F0-2A9E9B68C043}">
   <dimension ref="A1:B416"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A411" workbookViewId="0">
+    <sheetView topLeftCell="A411" workbookViewId="0">
       <selection activeCell="A417" activeCellId="1" sqref="A416:XFD416 A417:XFD417"/>
     </sheetView>
   </sheetViews>
@@ -10807,4 +10808,4028 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F259C1BD-E63C-4181-BBE6-486DED479F43}">
+  <dimension ref="A1:B501"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A495" workbookViewId="0">
+      <selection activeCell="C503" sqref="C503"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>0.1</v>
+      </c>
+      <c r="B2">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>0.2</v>
+      </c>
+      <c r="B3">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>0.3</v>
+      </c>
+      <c r="B4">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>0.4</v>
+      </c>
+      <c r="B5">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>0.5</v>
+      </c>
+      <c r="B6">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>0.6</v>
+      </c>
+      <c r="B7">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>0.7</v>
+      </c>
+      <c r="B8">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>0.8</v>
+      </c>
+      <c r="B9">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>0.9</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>1.2</v>
+      </c>
+      <c r="B13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>1.3</v>
+      </c>
+      <c r="B14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>1.4</v>
+      </c>
+      <c r="B15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>1.5</v>
+      </c>
+      <c r="B16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>1.6</v>
+      </c>
+      <c r="B17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>1.7</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>1.8</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>1.9</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>2.1</v>
+      </c>
+      <c r="B22">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B23">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B24">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>2.4</v>
+      </c>
+      <c r="B25">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>2.5</v>
+      </c>
+      <c r="B26">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>2.6</v>
+      </c>
+      <c r="B27">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>2.7</v>
+      </c>
+      <c r="B28">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>2.8</v>
+      </c>
+      <c r="B29">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>2.9</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>3</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>3.1</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>3.2</v>
+      </c>
+      <c r="B33">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>3.3</v>
+      </c>
+      <c r="B34">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>3.4</v>
+      </c>
+      <c r="B35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>3.5</v>
+      </c>
+      <c r="B36">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>3.6</v>
+      </c>
+      <c r="B37">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>3.7</v>
+      </c>
+      <c r="B38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>3.8</v>
+      </c>
+      <c r="B39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>3.9</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>4</v>
+      </c>
+      <c r="B41">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B42">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>4.2</v>
+      </c>
+      <c r="B43">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>4.3</v>
+      </c>
+      <c r="B44">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="B45">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>4.5</v>
+      </c>
+      <c r="B46">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="B47">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>4.7</v>
+      </c>
+      <c r="B48">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>4.8</v>
+      </c>
+      <c r="B49">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>5</v>
+      </c>
+      <c r="B51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B52">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>5.2</v>
+      </c>
+      <c r="B53">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <v>5.3</v>
+      </c>
+      <c r="B54">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A55">
+        <v>5.4</v>
+      </c>
+      <c r="B55">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A56">
+        <v>5.5</v>
+      </c>
+      <c r="B56">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A57">
+        <v>5.6</v>
+      </c>
+      <c r="B57">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A58">
+        <v>5.7</v>
+      </c>
+      <c r="B58">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A59">
+        <v>5.8</v>
+      </c>
+      <c r="B59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A60">
+        <v>5.9</v>
+      </c>
+      <c r="B60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A61">
+        <v>6</v>
+      </c>
+      <c r="B61">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A62">
+        <v>6.1</v>
+      </c>
+      <c r="B62">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A63">
+        <v>6.2</v>
+      </c>
+      <c r="B63">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A64">
+        <v>6.3</v>
+      </c>
+      <c r="B64">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A65">
+        <v>6.4</v>
+      </c>
+      <c r="B65">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A66">
+        <v>6.5</v>
+      </c>
+      <c r="B66">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A67">
+        <v>6.6</v>
+      </c>
+      <c r="B67">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A68">
+        <v>6.7</v>
+      </c>
+      <c r="B68">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A69">
+        <v>6.8</v>
+      </c>
+      <c r="B69">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A70">
+        <v>6.9</v>
+      </c>
+      <c r="B70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A71">
+        <v>7</v>
+      </c>
+      <c r="B71">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A72">
+        <v>7.1</v>
+      </c>
+      <c r="B72">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A73">
+        <v>7.2</v>
+      </c>
+      <c r="B73">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A74">
+        <v>7.3</v>
+      </c>
+      <c r="B74">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A75">
+        <v>7.4</v>
+      </c>
+      <c r="B75">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A76">
+        <v>7.5</v>
+      </c>
+      <c r="B76">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A77">
+        <v>7.6</v>
+      </c>
+      <c r="B77">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A78">
+        <v>7.7</v>
+      </c>
+      <c r="B78">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A79">
+        <v>7.8</v>
+      </c>
+      <c r="B79">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A80">
+        <v>7.9</v>
+      </c>
+      <c r="B80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A81">
+        <v>8</v>
+      </c>
+      <c r="B81">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A82">
+        <v>8.1</v>
+      </c>
+      <c r="B82">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A83">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="B83">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A84">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="B84">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A85">
+        <v>8.4</v>
+      </c>
+      <c r="B85">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A86">
+        <v>8.5</v>
+      </c>
+      <c r="B86">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A87">
+        <v>8.6</v>
+      </c>
+      <c r="B87">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A88">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="B88">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A89">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="B89">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A90">
+        <v>8.9</v>
+      </c>
+      <c r="B90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A91">
+        <v>9</v>
+      </c>
+      <c r="B91">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A92">
+        <v>9.1</v>
+      </c>
+      <c r="B92">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A93">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="B93">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A94">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="B94">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A95">
+        <v>9.4</v>
+      </c>
+      <c r="B95">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A96">
+        <v>9.5</v>
+      </c>
+      <c r="B96">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A97">
+        <v>9.6</v>
+      </c>
+      <c r="B97">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A98">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="B98">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A99">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="B99">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A100">
+        <v>9.9</v>
+      </c>
+      <c r="B100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A101">
+        <v>10</v>
+      </c>
+      <c r="B101">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A102">
+        <v>10.1</v>
+      </c>
+      <c r="B102">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A103">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="B103">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A104">
+        <v>10.3</v>
+      </c>
+      <c r="B104">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A105">
+        <v>10.4</v>
+      </c>
+      <c r="B105">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A106">
+        <v>10.5</v>
+      </c>
+      <c r="B106">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A107">
+        <v>10.6</v>
+      </c>
+      <c r="B107">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A108">
+        <v>10.7</v>
+      </c>
+      <c r="B108">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A109">
+        <v>10.8</v>
+      </c>
+      <c r="B109">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A110">
+        <v>10.9</v>
+      </c>
+      <c r="B110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A111">
+        <v>11</v>
+      </c>
+      <c r="B111">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A112">
+        <v>11.1</v>
+      </c>
+      <c r="B112">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A113">
+        <v>11.2</v>
+      </c>
+      <c r="B113">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A114">
+        <v>11.3</v>
+      </c>
+      <c r="B114">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A115">
+        <v>11.4</v>
+      </c>
+      <c r="B115">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A116">
+        <v>11.5</v>
+      </c>
+      <c r="B116">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A117">
+        <v>11.6</v>
+      </c>
+      <c r="B117">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A118">
+        <v>11.7</v>
+      </c>
+      <c r="B118">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A119">
+        <v>11.8</v>
+      </c>
+      <c r="B119">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A120">
+        <v>11.9</v>
+      </c>
+      <c r="B120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A121">
+        <v>12</v>
+      </c>
+      <c r="B121">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A122">
+        <v>12.1</v>
+      </c>
+      <c r="B122">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A123">
+        <v>12.2</v>
+      </c>
+      <c r="B123">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A124">
+        <v>12.3</v>
+      </c>
+      <c r="B124">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A125">
+        <v>12.4</v>
+      </c>
+      <c r="B125">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A126">
+        <v>12.5</v>
+      </c>
+      <c r="B126">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A127">
+        <v>12.6</v>
+      </c>
+      <c r="B127">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A128">
+        <v>12.7</v>
+      </c>
+      <c r="B128">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A129">
+        <v>12.8</v>
+      </c>
+      <c r="B129">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A130">
+        <v>12.9</v>
+      </c>
+      <c r="B130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A131">
+        <v>13</v>
+      </c>
+      <c r="B131">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A132">
+        <v>13.1</v>
+      </c>
+      <c r="B132">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A133">
+        <v>13.2</v>
+      </c>
+      <c r="B133">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A134">
+        <v>13.3</v>
+      </c>
+      <c r="B134">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A135">
+        <v>13.4</v>
+      </c>
+      <c r="B135">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A136">
+        <v>13.5</v>
+      </c>
+      <c r="B136">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A137">
+        <v>13.6</v>
+      </c>
+      <c r="B137">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A138">
+        <v>13.7</v>
+      </c>
+      <c r="B138">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A139">
+        <v>13.8</v>
+      </c>
+      <c r="B139">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A140">
+        <v>13.9</v>
+      </c>
+      <c r="B140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A141">
+        <v>14</v>
+      </c>
+      <c r="B141">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A142">
+        <v>14.1</v>
+      </c>
+      <c r="B142">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A143">
+        <v>14.2</v>
+      </c>
+      <c r="B143">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A144">
+        <v>14.3</v>
+      </c>
+      <c r="B144">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A145">
+        <v>14.4</v>
+      </c>
+      <c r="B145">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A146">
+        <v>14.5</v>
+      </c>
+      <c r="B146">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A147">
+        <v>14.6</v>
+      </c>
+      <c r="B147">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A148">
+        <v>14.7</v>
+      </c>
+      <c r="B148">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A149">
+        <v>14.8</v>
+      </c>
+      <c r="B149">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A150">
+        <v>14.9</v>
+      </c>
+      <c r="B150">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A151">
+        <v>15</v>
+      </c>
+      <c r="B151">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A152">
+        <v>15.1</v>
+      </c>
+      <c r="B152">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A153">
+        <v>15.2</v>
+      </c>
+      <c r="B153">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A154">
+        <v>15.3</v>
+      </c>
+      <c r="B154">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A155">
+        <v>15.4</v>
+      </c>
+      <c r="B155">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A156">
+        <v>15.5</v>
+      </c>
+      <c r="B156">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A157">
+        <v>15.6</v>
+      </c>
+      <c r="B157">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A158">
+        <v>15.7</v>
+      </c>
+      <c r="B158">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A159">
+        <v>15.8</v>
+      </c>
+      <c r="B159">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A160">
+        <v>15.9</v>
+      </c>
+      <c r="B160">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A161">
+        <v>16</v>
+      </c>
+      <c r="B161">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A162">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="B162">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A163">
+        <v>16.2</v>
+      </c>
+      <c r="B163">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A164">
+        <v>16.3</v>
+      </c>
+      <c r="B164">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A165">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="B165">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A166">
+        <v>16.5</v>
+      </c>
+      <c r="B166">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A167">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="B167">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A168">
+        <v>16.7</v>
+      </c>
+      <c r="B168">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A169">
+        <v>16.8</v>
+      </c>
+      <c r="B169">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A170">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="B170">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A171">
+        <v>17</v>
+      </c>
+      <c r="B171">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A172">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="B172">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A173">
+        <v>17.2</v>
+      </c>
+      <c r="B173">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A174">
+        <v>17.3</v>
+      </c>
+      <c r="B174">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A175">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="B175">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A176">
+        <v>17.5</v>
+      </c>
+      <c r="B176">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A177">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="B177">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A178">
+        <v>17.7</v>
+      </c>
+      <c r="B178">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A179">
+        <v>17.8</v>
+      </c>
+      <c r="B179">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A180">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="B180">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A181">
+        <v>18</v>
+      </c>
+      <c r="B181">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A182">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="B182">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A183">
+        <v>18.2</v>
+      </c>
+      <c r="B183">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A184">
+        <v>18.3</v>
+      </c>
+      <c r="B184">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A185">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="B185">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A186">
+        <v>18.5</v>
+      </c>
+      <c r="B186">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A187">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="B187">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A188">
+        <v>18.7</v>
+      </c>
+      <c r="B188">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A189">
+        <v>18.8</v>
+      </c>
+      <c r="B189">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A190">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="B190">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A191">
+        <v>19</v>
+      </c>
+      <c r="B191">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A192">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="B192">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A193">
+        <v>19.2</v>
+      </c>
+      <c r="B193">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A194">
+        <v>19.3</v>
+      </c>
+      <c r="B194">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A195">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="B195">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A196">
+        <v>19.5</v>
+      </c>
+      <c r="B196">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A197">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="B197">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A198">
+        <v>19.7</v>
+      </c>
+      <c r="B198">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A199">
+        <v>19.8</v>
+      </c>
+      <c r="B199">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A200">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="B200">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A201">
+        <v>20</v>
+      </c>
+      <c r="B201">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A202">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="B202">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A203">
+        <v>20.2</v>
+      </c>
+      <c r="B203">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A204">
+        <v>20.3</v>
+      </c>
+      <c r="B204">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A205">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="B205">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A206">
+        <v>20.5</v>
+      </c>
+      <c r="B206">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A207">
+        <v>20.6</v>
+      </c>
+      <c r="B207">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A208">
+        <v>20.7</v>
+      </c>
+      <c r="B208">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A209">
+        <v>20.8</v>
+      </c>
+      <c r="B209">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A210">
+        <v>20.9</v>
+      </c>
+      <c r="B210">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A211">
+        <v>21</v>
+      </c>
+      <c r="B211">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A212">
+        <v>21.1</v>
+      </c>
+      <c r="B212">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A213">
+        <v>21.2</v>
+      </c>
+      <c r="B213">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A214">
+        <v>21.3</v>
+      </c>
+      <c r="B214">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A215">
+        <v>21.4</v>
+      </c>
+      <c r="B215">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A216">
+        <v>21.5</v>
+      </c>
+      <c r="B216">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A217">
+        <v>21.6</v>
+      </c>
+      <c r="B217">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A218">
+        <v>21.7</v>
+      </c>
+      <c r="B218">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A219">
+        <v>21.8</v>
+      </c>
+      <c r="B219">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A220">
+        <v>21.9</v>
+      </c>
+      <c r="B220">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A221">
+        <v>22</v>
+      </c>
+      <c r="B221">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A222">
+        <v>22.1</v>
+      </c>
+      <c r="B222">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A223">
+        <v>22.2</v>
+      </c>
+      <c r="B223">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A224">
+        <v>22.3</v>
+      </c>
+      <c r="B224">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A225">
+        <v>22.4</v>
+      </c>
+      <c r="B225">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A226">
+        <v>22.5</v>
+      </c>
+      <c r="B226">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A227">
+        <v>22.6</v>
+      </c>
+      <c r="B227">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A228">
+        <v>22.7</v>
+      </c>
+      <c r="B228">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A229">
+        <v>22.8</v>
+      </c>
+      <c r="B229">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A230">
+        <v>22.9</v>
+      </c>
+      <c r="B230">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A231">
+        <v>23</v>
+      </c>
+      <c r="B231">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A232">
+        <v>23.1</v>
+      </c>
+      <c r="B232">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A233">
+        <v>23.2</v>
+      </c>
+      <c r="B233">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A234">
+        <v>23.3</v>
+      </c>
+      <c r="B234">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A235">
+        <v>23.4</v>
+      </c>
+      <c r="B235">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A236">
+        <v>23.5</v>
+      </c>
+      <c r="B236">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A237">
+        <v>23.6</v>
+      </c>
+      <c r="B237">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A238">
+        <v>23.7</v>
+      </c>
+      <c r="B238">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A239">
+        <v>23.8</v>
+      </c>
+      <c r="B239">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A240">
+        <v>23.9</v>
+      </c>
+      <c r="B240">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A241">
+        <v>24</v>
+      </c>
+      <c r="B241">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A242">
+        <v>24.1</v>
+      </c>
+      <c r="B242">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A243">
+        <v>24.2</v>
+      </c>
+      <c r="B243">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A244">
+        <v>24.3</v>
+      </c>
+      <c r="B244">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A245">
+        <v>24.4</v>
+      </c>
+      <c r="B245">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A246">
+        <v>24.5</v>
+      </c>
+      <c r="B246">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A247">
+        <v>24.6</v>
+      </c>
+      <c r="B247">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A248">
+        <v>24.7</v>
+      </c>
+      <c r="B248">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A249">
+        <v>24.8</v>
+      </c>
+      <c r="B249">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A250">
+        <v>24.9</v>
+      </c>
+      <c r="B250">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A251">
+        <v>25</v>
+      </c>
+      <c r="B251">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A252">
+        <v>25.1</v>
+      </c>
+      <c r="B252">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A253">
+        <v>25.2</v>
+      </c>
+      <c r="B253">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A254">
+        <v>25.3</v>
+      </c>
+      <c r="B254">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A255">
+        <v>25.4</v>
+      </c>
+      <c r="B255">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A256">
+        <v>25.5</v>
+      </c>
+      <c r="B256">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A257">
+        <v>25.6</v>
+      </c>
+      <c r="B257">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A258">
+        <v>25.7</v>
+      </c>
+      <c r="B258">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A259">
+        <v>25.8</v>
+      </c>
+      <c r="B259">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A260">
+        <v>25.9</v>
+      </c>
+      <c r="B260">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A261">
+        <v>26</v>
+      </c>
+      <c r="B261">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A262">
+        <v>26.1</v>
+      </c>
+      <c r="B262">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A263">
+        <v>26.2</v>
+      </c>
+      <c r="B263">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A264">
+        <v>26.3</v>
+      </c>
+      <c r="B264">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A265">
+        <v>26.4</v>
+      </c>
+      <c r="B265">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A266">
+        <v>26.5</v>
+      </c>
+      <c r="B266">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A267">
+        <v>26.6</v>
+      </c>
+      <c r="B267">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A268">
+        <v>26.7</v>
+      </c>
+      <c r="B268">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A269">
+        <v>26.8</v>
+      </c>
+      <c r="B269">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A270">
+        <v>26.9</v>
+      </c>
+      <c r="B270">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A271">
+        <v>27</v>
+      </c>
+      <c r="B271">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A272">
+        <v>27.1</v>
+      </c>
+      <c r="B272">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A273">
+        <v>27.2</v>
+      </c>
+      <c r="B273">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A274">
+        <v>27.3</v>
+      </c>
+      <c r="B274">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A275">
+        <v>27.4</v>
+      </c>
+      <c r="B275">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A276">
+        <v>27.5</v>
+      </c>
+      <c r="B276">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A277">
+        <v>27.6</v>
+      </c>
+      <c r="B277">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A278">
+        <v>27.7</v>
+      </c>
+      <c r="B278">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A279">
+        <v>27.8</v>
+      </c>
+      <c r="B279">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A280">
+        <v>27.9</v>
+      </c>
+      <c r="B280">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A281">
+        <v>28</v>
+      </c>
+      <c r="B281">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A282">
+        <v>28.1</v>
+      </c>
+      <c r="B282">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A283">
+        <v>28.2</v>
+      </c>
+      <c r="B283">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A284">
+        <v>28.3</v>
+      </c>
+      <c r="B284">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A285">
+        <v>28.4</v>
+      </c>
+      <c r="B285">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A286">
+        <v>28.5</v>
+      </c>
+      <c r="B286">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A287">
+        <v>28.6</v>
+      </c>
+      <c r="B287">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A288">
+        <v>28.7</v>
+      </c>
+      <c r="B288">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A289">
+        <v>28.8</v>
+      </c>
+      <c r="B289">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A290">
+        <v>28.9</v>
+      </c>
+      <c r="B290">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A291">
+        <v>29</v>
+      </c>
+      <c r="B291">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A292">
+        <v>29.1</v>
+      </c>
+      <c r="B292">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A293">
+        <v>29.2</v>
+      </c>
+      <c r="B293">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A294">
+        <v>29.3</v>
+      </c>
+      <c r="B294">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A295">
+        <v>29.4</v>
+      </c>
+      <c r="B295">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A296">
+        <v>29.5</v>
+      </c>
+      <c r="B296">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A297">
+        <v>29.6</v>
+      </c>
+      <c r="B297">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A298">
+        <v>29.7</v>
+      </c>
+      <c r="B298">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A299">
+        <v>29.8</v>
+      </c>
+      <c r="B299">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A300">
+        <v>29.9</v>
+      </c>
+      <c r="B300">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A301">
+        <v>30</v>
+      </c>
+      <c r="B301">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A302">
+        <v>30.1</v>
+      </c>
+      <c r="B302">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="303" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A303">
+        <v>30.2</v>
+      </c>
+      <c r="B303">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A304">
+        <v>30.3</v>
+      </c>
+      <c r="B304">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="305" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A305">
+        <v>30.4</v>
+      </c>
+      <c r="B305">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="306" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A306">
+        <v>30.5</v>
+      </c>
+      <c r="B306">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="307" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A307">
+        <v>30.6</v>
+      </c>
+      <c r="B307">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="308" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A308">
+        <v>30.7</v>
+      </c>
+      <c r="B308">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="309" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A309">
+        <v>30.8</v>
+      </c>
+      <c r="B309">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="310" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A310">
+        <v>30.9</v>
+      </c>
+      <c r="B310">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="311" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A311">
+        <v>31</v>
+      </c>
+      <c r="B311">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="312" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A312">
+        <v>31.1</v>
+      </c>
+      <c r="B312">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="313" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A313">
+        <v>31.2</v>
+      </c>
+      <c r="B313">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="314" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A314">
+        <v>31.3</v>
+      </c>
+      <c r="B314">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="315" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A315">
+        <v>31.4</v>
+      </c>
+      <c r="B315">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="316" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A316">
+        <v>31.5</v>
+      </c>
+      <c r="B316">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="317" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A317">
+        <v>31.6</v>
+      </c>
+      <c r="B317">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="318" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A318">
+        <v>31.7</v>
+      </c>
+      <c r="B318">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="319" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A319">
+        <v>31.8</v>
+      </c>
+      <c r="B319">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="320" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A320">
+        <v>31.9</v>
+      </c>
+      <c r="B320">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="321" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A321">
+        <v>32</v>
+      </c>
+      <c r="B321">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="322" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A322">
+        <v>32.1</v>
+      </c>
+      <c r="B322">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="323" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A323">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="B323">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="324" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A324">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="B324">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="325" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A325">
+        <v>32.4</v>
+      </c>
+      <c r="B325">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="326" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A326">
+        <v>32.5</v>
+      </c>
+      <c r="B326">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="327" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A327">
+        <v>32.6</v>
+      </c>
+      <c r="B327">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A328">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="B328">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="329" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A329">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="B329">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="330" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A330">
+        <v>32.9</v>
+      </c>
+      <c r="B330">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="331" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A331">
+        <v>33</v>
+      </c>
+      <c r="B331">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="332" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A332">
+        <v>33.1</v>
+      </c>
+      <c r="B332">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="333" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A333">
+        <v>33.200000000000003</v>
+      </c>
+      <c r="B333">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="334" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A334">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="B334">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="335" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A335">
+        <v>33.4</v>
+      </c>
+      <c r="B335">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A336">
+        <v>33.5</v>
+      </c>
+      <c r="B336">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="337" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A337">
+        <v>33.6</v>
+      </c>
+      <c r="B337">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="338" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A338">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="B338">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="339" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A339">
+        <v>33.799999999999997</v>
+      </c>
+      <c r="B339">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="340" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A340">
+        <v>33.9</v>
+      </c>
+      <c r="B340">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="341" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A341">
+        <v>34</v>
+      </c>
+      <c r="B341">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="342" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A342">
+        <v>34.1</v>
+      </c>
+      <c r="B342">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="343" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A343">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="B343">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A344">
+        <v>34.299999999999997</v>
+      </c>
+      <c r="B344">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="345" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A345">
+        <v>34.4</v>
+      </c>
+      <c r="B345">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="346" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A346">
+        <v>34.5</v>
+      </c>
+      <c r="B346">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="347" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A347">
+        <v>34.6</v>
+      </c>
+      <c r="B347">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="348" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A348">
+        <v>34.700000000000003</v>
+      </c>
+      <c r="B348">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="349" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A349">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="B349">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A350">
+        <v>34.9</v>
+      </c>
+      <c r="B350">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="351" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A351">
+        <v>35</v>
+      </c>
+      <c r="B351">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="352" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A352">
+        <v>35.1</v>
+      </c>
+      <c r="B352">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="353" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A353">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="B353">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="354" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A354">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="B354">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="355" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A355">
+        <v>35.4</v>
+      </c>
+      <c r="B355">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="356" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A356">
+        <v>35.5</v>
+      </c>
+      <c r="B356">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="357" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A357">
+        <v>35.6</v>
+      </c>
+      <c r="B357">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="358" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A358">
+        <v>35.700000000000003</v>
+      </c>
+      <c r="B358">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="359" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A359">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="B359">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="360" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A360">
+        <v>35.9</v>
+      </c>
+      <c r="B360">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="361" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A361">
+        <v>36</v>
+      </c>
+      <c r="B361">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="362" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A362">
+        <v>36.1</v>
+      </c>
+      <c r="B362">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="363" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A363">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="B363">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="364" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A364">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="B364">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="365" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A365">
+        <v>36.4</v>
+      </c>
+      <c r="B365">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="366" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A366">
+        <v>36.5</v>
+      </c>
+      <c r="B366">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="367" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A367">
+        <v>36.6</v>
+      </c>
+      <c r="B367">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="368" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A368">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="B368">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="369" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A369">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="B369">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="370" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A370">
+        <v>36.9</v>
+      </c>
+      <c r="B370">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="371" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A371">
+        <v>37</v>
+      </c>
+      <c r="B371">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="372" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A372">
+        <v>37.1</v>
+      </c>
+      <c r="B372">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="373" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A373">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="B373">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="374" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A374">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="B374">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="375" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A375">
+        <v>37.4</v>
+      </c>
+      <c r="B375">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="376" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A376">
+        <v>37.5</v>
+      </c>
+      <c r="B376">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="377" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A377">
+        <v>37.6</v>
+      </c>
+      <c r="B377">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="378" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A378">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="B378">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="379" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A379">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="B379">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="380" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A380">
+        <v>37.9</v>
+      </c>
+      <c r="B380">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="381" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A381">
+        <v>38</v>
+      </c>
+      <c r="B381">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="382" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A382">
+        <v>38.1</v>
+      </c>
+      <c r="B382">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="383" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A383">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="B383">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="384" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A384">
+        <v>38.299999999999997</v>
+      </c>
+      <c r="B384">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="385" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A385">
+        <v>38.4</v>
+      </c>
+      <c r="B385">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="386" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A386">
+        <v>38.5</v>
+      </c>
+      <c r="B386">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="387" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A387">
+        <v>38.6</v>
+      </c>
+      <c r="B387">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="388" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A388">
+        <v>38.700000000000003</v>
+      </c>
+      <c r="B388">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="389" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A389">
+        <v>38.799999999999997</v>
+      </c>
+      <c r="B389">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="390" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A390">
+        <v>38.9</v>
+      </c>
+      <c r="B390">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="391" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A391">
+        <v>39</v>
+      </c>
+      <c r="B391">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="392" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A392">
+        <v>39.1</v>
+      </c>
+      <c r="B392">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="393" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A393">
+        <v>39.200000000000003</v>
+      </c>
+      <c r="B393">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="394" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A394">
+        <v>39.299999999999997</v>
+      </c>
+      <c r="B394">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="395" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A395">
+        <v>39.4</v>
+      </c>
+      <c r="B395">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="396" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A396">
+        <v>39.5</v>
+      </c>
+      <c r="B396">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="397" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A397">
+        <v>39.6</v>
+      </c>
+      <c r="B397">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="398" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A398">
+        <v>39.700000000000003</v>
+      </c>
+      <c r="B398">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="399" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A399">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="B399">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="400" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A400">
+        <v>39.9</v>
+      </c>
+      <c r="B400">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="401" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A401">
+        <v>40</v>
+      </c>
+      <c r="B401">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="402" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A402">
+        <v>40.1</v>
+      </c>
+      <c r="B402">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="403" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A403">
+        <v>40.200000000000003</v>
+      </c>
+      <c r="B403">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="404" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A404">
+        <v>40.299999999999997</v>
+      </c>
+      <c r="B404">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="405" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A405">
+        <v>40.4</v>
+      </c>
+      <c r="B405">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="406" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A406">
+        <v>40.5</v>
+      </c>
+      <c r="B406">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="407" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A407">
+        <v>40.6</v>
+      </c>
+      <c r="B407">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="408" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A408">
+        <v>40.700000000000003</v>
+      </c>
+      <c r="B408">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="409" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A409">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="B409">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="410" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A410">
+        <v>40.9</v>
+      </c>
+      <c r="B410">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="411" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A411">
+        <v>41</v>
+      </c>
+      <c r="B411">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="412" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A412">
+        <v>41.1</v>
+      </c>
+      <c r="B412">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="413" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A413">
+        <v>41.2</v>
+      </c>
+      <c r="B413">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="414" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A414">
+        <v>41.3</v>
+      </c>
+      <c r="B414">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="415" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A415">
+        <v>41.4</v>
+      </c>
+      <c r="B415">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="416" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A416">
+        <v>41.5</v>
+      </c>
+      <c r="B416">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="417" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A417">
+        <v>41.6</v>
+      </c>
+      <c r="B417">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="418" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A418">
+        <v>41.7</v>
+      </c>
+      <c r="B418">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="419" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A419">
+        <v>41.8</v>
+      </c>
+      <c r="B419">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="420" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A420">
+        <v>41.9</v>
+      </c>
+      <c r="B420">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="421" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A421">
+        <v>42</v>
+      </c>
+      <c r="B421">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="422" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A422">
+        <v>42.1</v>
+      </c>
+      <c r="B422">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="423" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A423">
+        <v>42.2</v>
+      </c>
+      <c r="B423">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="424" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A424">
+        <v>42.3</v>
+      </c>
+      <c r="B424">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="425" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A425">
+        <v>42.4</v>
+      </c>
+      <c r="B425">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="426" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A426">
+        <v>42.5</v>
+      </c>
+      <c r="B426">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="427" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A427">
+        <v>42.6</v>
+      </c>
+      <c r="B427">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="428" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A428">
+        <v>42.7</v>
+      </c>
+      <c r="B428">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="429" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A429">
+        <v>42.8</v>
+      </c>
+      <c r="B429">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="430" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A430">
+        <v>42.9</v>
+      </c>
+      <c r="B430">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="431" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A431">
+        <v>43</v>
+      </c>
+      <c r="B431">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="432" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A432">
+        <v>43.1</v>
+      </c>
+      <c r="B432">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="433" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A433">
+        <v>43.2</v>
+      </c>
+      <c r="B433">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="434" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A434">
+        <v>43.3</v>
+      </c>
+      <c r="B434">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="435" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A435">
+        <v>43.4</v>
+      </c>
+      <c r="B435">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="436" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A436">
+        <v>43.5</v>
+      </c>
+      <c r="B436">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="437" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A437">
+        <v>43.6</v>
+      </c>
+      <c r="B437">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="438" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A438">
+        <v>43.7</v>
+      </c>
+      <c r="B438">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="439" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A439">
+        <v>43.8</v>
+      </c>
+      <c r="B439">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="440" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A440">
+        <v>43.9</v>
+      </c>
+      <c r="B440">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="441" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A441">
+        <v>44</v>
+      </c>
+      <c r="B441">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="442" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A442">
+        <v>44.1</v>
+      </c>
+      <c r="B442">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="443" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A443">
+        <v>44.2</v>
+      </c>
+      <c r="B443">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="444" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A444">
+        <v>44.3</v>
+      </c>
+      <c r="B444">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="445" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A445">
+        <v>44.4</v>
+      </c>
+      <c r="B445">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="446" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A446">
+        <v>44.5</v>
+      </c>
+      <c r="B446">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="447" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A447">
+        <v>44.6</v>
+      </c>
+      <c r="B447">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="448" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A448">
+        <v>44.7</v>
+      </c>
+      <c r="B448">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="449" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A449">
+        <v>44.8</v>
+      </c>
+      <c r="B449">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="450" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A450">
+        <v>44.9</v>
+      </c>
+      <c r="B450">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="451" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A451">
+        <v>45</v>
+      </c>
+      <c r="B451">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="452" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A452">
+        <v>45.1</v>
+      </c>
+      <c r="B452">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="453" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A453">
+        <v>45.2</v>
+      </c>
+      <c r="B453">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="454" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A454">
+        <v>45.3</v>
+      </c>
+      <c r="B454">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="455" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A455">
+        <v>45.4</v>
+      </c>
+      <c r="B455">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="456" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A456">
+        <v>45.5</v>
+      </c>
+      <c r="B456">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="457" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A457">
+        <v>45.6</v>
+      </c>
+      <c r="B457">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="458" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A458">
+        <v>45.7</v>
+      </c>
+      <c r="B458">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="459" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A459">
+        <v>45.8</v>
+      </c>
+      <c r="B459">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="460" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A460">
+        <v>45.9</v>
+      </c>
+      <c r="B460">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="461" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A461">
+        <v>46</v>
+      </c>
+      <c r="B461">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="462" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A462">
+        <v>46.1</v>
+      </c>
+      <c r="B462">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="463" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A463">
+        <v>46.2</v>
+      </c>
+      <c r="B463">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="464" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A464">
+        <v>46.3</v>
+      </c>
+      <c r="B464">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="465" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A465">
+        <v>46.4</v>
+      </c>
+      <c r="B465">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="466" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A466">
+        <v>46.5</v>
+      </c>
+      <c r="B466">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="467" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A467">
+        <v>46.6</v>
+      </c>
+      <c r="B467">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="468" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A468">
+        <v>46.7</v>
+      </c>
+      <c r="B468">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="469" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A469">
+        <v>46.8</v>
+      </c>
+      <c r="B469">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="470" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A470">
+        <v>46.9</v>
+      </c>
+      <c r="B470">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="471" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A471">
+        <v>47</v>
+      </c>
+      <c r="B471">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="472" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A472">
+        <v>47.1</v>
+      </c>
+      <c r="B472">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="473" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A473">
+        <v>47.2</v>
+      </c>
+      <c r="B473">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="474" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A474">
+        <v>47.3</v>
+      </c>
+      <c r="B474">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="475" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A475">
+        <v>47.4</v>
+      </c>
+      <c r="B475">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="476" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A476">
+        <v>47.5</v>
+      </c>
+      <c r="B476">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="477" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A477">
+        <v>47.6</v>
+      </c>
+      <c r="B477">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="478" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A478">
+        <v>47.7</v>
+      </c>
+      <c r="B478">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="479" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A479">
+        <v>47.8</v>
+      </c>
+      <c r="B479">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="480" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A480">
+        <v>47.9</v>
+      </c>
+      <c r="B480">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="481" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A481">
+        <v>48</v>
+      </c>
+      <c r="B481">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="482" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A482">
+        <v>48.1</v>
+      </c>
+      <c r="B482">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="483" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A483">
+        <v>48.2</v>
+      </c>
+      <c r="B483">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="484" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A484">
+        <v>48.3</v>
+      </c>
+      <c r="B484">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="485" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A485">
+        <v>48.4</v>
+      </c>
+      <c r="B485">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="486" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A486">
+        <v>48.5</v>
+      </c>
+      <c r="B486">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="487" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A487">
+        <v>48.6</v>
+      </c>
+      <c r="B487">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="488" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A488">
+        <v>48.7</v>
+      </c>
+      <c r="B488">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="489" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A489">
+        <v>48.8</v>
+      </c>
+      <c r="B489">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="490" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A490">
+        <v>48.9</v>
+      </c>
+      <c r="B490">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="491" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A491">
+        <v>49</v>
+      </c>
+      <c r="B491">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="492" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A492">
+        <v>49.1</v>
+      </c>
+      <c r="B492">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="493" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A493">
+        <v>49.2</v>
+      </c>
+      <c r="B493">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="494" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A494">
+        <v>49.3</v>
+      </c>
+      <c r="B494">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="495" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A495">
+        <v>49.4</v>
+      </c>
+      <c r="B495">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="496" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A496">
+        <v>49.5</v>
+      </c>
+      <c r="B496">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="497" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A497">
+        <v>49.6</v>
+      </c>
+      <c r="B497">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="498" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A498">
+        <v>49.7</v>
+      </c>
+      <c r="B498">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="499" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A499">
+        <v>49.8</v>
+      </c>
+      <c r="B499">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="500" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A500">
+        <v>49.9</v>
+      </c>
+      <c r="B500">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="501" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A501">
+        <v>50</v>
+      </c>
+      <c r="B501">
+        <v>-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>